<commit_message>
Update giao diện, Usecase Format Chấm công
</commit_message>
<xml_diff>
--- a/Thiết kế/Thiết kế giao diện/Mẫn Đạt/Quản lí danh mục Khách hàng.xlsx
+++ b/Thiết kế/Thiết kế giao diện/Mẫn Đạt/Quản lí danh mục Khách hàng.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\CNPM\Thiết kế\Thiết kế giao diện\NgManDat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\CN Phan Mem\Homework\CNPM\Thiết kế\Thiết kế giao diện\Mẫn Đạt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA145C80-7483-45F3-9076-A8E0E58EF261}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A477BBED-2C50-44D9-A1E9-16111002BEF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93EB45F7-56C3-4B7A-8563-2AB1B894BB22}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{93EB45F7-56C3-4B7A-8563-2AB1B894BB22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,16 +484,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>973455</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EE36F1E-5900-4B46-896B-85D55D6CBC7D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3F8820E-1CF8-4A4F-A60D-0DABF3545021}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -517,7 +517,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9966960" cy="4419600"/>
+          <a:ext cx="9486900" cy="4122420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -838,24 +838,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9BE349-BC58-4389-A7FE-3D2DE67A1BE9}">
   <dimension ref="A27:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="8.88671875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>5</v>
       </c>
@@ -901,7 +901,7 @@
       </c>
       <c r="D30" s="9"/>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>2</v>
       </c>
@@ -913,7 +913,7 @@
       </c>
       <c r="D31" s="9"/>
     </row>
-    <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>3</v>
       </c>
@@ -949,7 +949,7 @@
       </c>
       <c r="D34" s="9"/>
     </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>6</v>
       </c>
@@ -973,7 +973,7 @@
       </c>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11">
         <v>8</v>
       </c>
@@ -990,7 +990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>6</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="F57" s="4"/>
       <c r="G57" s="9"/>
     </row>
-    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11">
         <v>18</v>
       </c>

</xml_diff>